<commit_message>
Added import Excel initial solution table
</commit_message>
<xml_diff>
--- a/example/example1.xlsx
+++ b/example/example1.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
-  <si>
-    <t>1.8</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>H</t>
   </si>
@@ -45,6 +42,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -87,7 +87,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -407,23 +407,23 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -436,8 +436,8 @@
       <c r="C2" s="2">
         <v>700</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>0</v>
+      <c r="D2" s="2">
+        <v>1.8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -450,8 +450,8 @@
       <c r="C3" s="2">
         <v>700</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>0</v>
+      <c r="D3" s="2">
+        <v>1.8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -464,8 +464,8 @@
       <c r="C4" s="2">
         <v>700</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>0</v>
+      <c r="D4" s="2">
+        <v>1.8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -476,11 +476,12 @@
       <c r="C5" s="2">
         <v>700</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>0</v>
+      <c r="D5" s="2">
+        <v>1.8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added load of dispertion curve from Excel
</commit_message>
<xml_diff>
--- a/example/example1.xlsx
+++ b/example/example1.xlsx
@@ -29,13 +29,13 @@
     <t>H</t>
   </si>
   <si>
-    <t>Vs</t>
+    <t>VS</t>
   </si>
   <si>
-    <t>Vp</t>
+    <t>VP</t>
   </si>
   <si>
-    <t>ρ</t>
+    <t>RHO</t>
   </si>
 </sst>
 </file>
@@ -45,16 +45,8 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -84,10 +76,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -407,76 +399,76 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>5</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>350</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>700</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>1.8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>5</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>350</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>700</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>1.8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>10</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>350</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>700</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>1.8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1">
         <v>350</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>700</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>1.8</v>
       </c>
     </row>

</xml_diff>